<commit_message>
Add Rewards processing (views not yet implemented)
</commit_message>
<xml_diff>
--- a/WarframeStatsSchemaData.xlsx
+++ b/WarframeStatsSchemaData.xlsx
@@ -1234,7 +1234,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1244,7 +1244,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>